<commit_message>
fixed encoding issue (molgenis-projects-rd-apps#2)
</commit_message>
<xml_diff>
--- a/data/ern_genturis_dataproviders.xlsx
+++ b/data/ern_genturis_dataproviders.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/molgenis-data-erns/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F7C6E538-B374-3C4F-9856-FA511CF45238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17E04AE-EC97-884B-A8A4-E1F6A3A7CC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-6860" windowWidth="38400" windowHeight="21100"/>
+    <workbookView xWindow="-38400" yWindow="-6860" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ernstats_dataproviders" sheetId="1" r:id="rId1"/>
@@ -721,7 +721,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1569,11 +1569,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3411,16 +3411,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1"/>
-    <hyperlink ref="I18" r:id="rId2"/>
-    <hyperlink ref="I23" r:id="rId3"/>
-    <hyperlink ref="I27" r:id="rId4"/>
-    <hyperlink ref="I44" r:id="rId5"/>
-    <hyperlink ref="I45" r:id="rId6"/>
-    <hyperlink ref="I35" r:id="rId7"/>
-    <hyperlink ref="I37" r:id="rId8"/>
-    <hyperlink ref="I38" r:id="rId9"/>
-    <hyperlink ref="I48" r:id="rId10"/>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="I23" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="I27" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="I44" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="I45" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="I35" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="I37" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="I38" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="I48" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>